<commit_message>
added remaining documents; added NSE logo to all docs
</commit_message>
<xml_diff>
--- a/10 Project Budget (Earned Value Analysis Report).xlsx
+++ b/10 Project Budget (Earned Value Analysis Report).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitrepos\NSE_new_product_launch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBB2D28-64EB-4418-85DF-BBD31A49C2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AD76C7-D19D-4517-BE29-8562896A3D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="20" windowWidth="23610" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="3" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="91">
   <si>
     <t>Earned Value Analysis Report</t>
   </si>
@@ -2198,6 +2198,51 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>62865</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247006</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>140996</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A608FB12-331A-4BD9-8B77-91F75BAAEE8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10648315" y="95250"/>
+          <a:ext cx="1371591" cy="299746"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2621,7 +2666,7 @@
   <dimension ref="A1:AF51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF44" sqref="AF44"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2647,6 +2692,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>2</v>
@@ -2665,7 +2715,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="51">
-        <v>46119</v>
+        <v>46054</v>
       </c>
       <c r="D5" s="52"/>
     </row>
@@ -4674,13 +4724,16 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="Q3" r:id="rId1" display="https://www.vertex42.com/ExcelTemplates/earned-value-management.html" xr:uid="{5B56347F-50A8-4C28-B420-66C874C7BB53}"/>
+  </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.25" bottom="0.5" header="0.5" footer="0.25"/>
-  <pageSetup scale="91" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="91" orientation="landscape" r:id="rId2"/>
   <headerFooter scaleWithDoc="0">
     <oddFooter>&amp;L&amp;8&amp;K01+049https://www.vertex42.com/ExcelTemplates/earned-value-management.html&amp;R&amp;8&amp;K01+049EVM Template © 2012 Vertex42 LLC</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>